<commit_message>
Feat: salva estado e porcentagem de estagiário
</commit_message>
<xml_diff>
--- a/Relatorio_Alocacao_2025-07-08.xlsx
+++ b/Relatorio_Alocacao_2025-07-08.xlsx
@@ -179,12 +179,138 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Lote 1'!$L$3:$L$7</f>
+              <f>'Consolidado'!$K$3:$K$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Lote 1'!$M$3:$M$7</f>
+              <f>'Consolidado'!$L$3:$L$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Total Decimal</v>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Lote 1'!$J$3:$J$5</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Lote 1'!$K$3:$K$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Total Decimal</v>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Lote 2'!$J$3:$J$5</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Lote 2'!$K$3:$K$5</f>
             </numRef>
           </val>
         </ser>
@@ -227,7 +353,61 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>14</row>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>11</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -537,7 +717,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,8 +731,7 @@
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="9" customWidth="1" min="8" max="8"/>
+    <col width="9" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -588,12 +767,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Apr/24</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
           <t>H.mês</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Fonte de Dados para o Gráfico</t>
         </is>
       </c>
     </row>
@@ -609,7 +788,16 @@
       <c r="E2" s="2" t="n"/>
       <c r="F2" s="2" t="n"/>
       <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Mês</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Total Decimal</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -624,33 +812,36 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>teste1</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>0,62</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>0,38</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>3,12</t>
-        </is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Cargo/Subcontrato</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -661,38 +852,41 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>testr1</t>
+          <t>teste3</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>0,34</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>1,91</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>1,56</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>3,12</t>
-        </is>
+          <t>3,81</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Jan/24</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>1.72</v>
       </c>
     </row>
     <row r="5">
@@ -707,7 +901,14 @@
       <c r="E5" s="2" t="n"/>
       <c r="F5" s="2" t="n"/>
       <c r="G5" s="2" t="n"/>
-      <c r="H5" s="2" t="n"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Feb/24</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>4.51</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -717,12 +918,12 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>teste7</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -732,145 +933,72 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>0,38</t>
+          <t>0,84</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>0,38</t>
+          <t>0,47</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>0,38</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>1,50</t>
-        </is>
+          <t>1,69</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Mar/24</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>2.79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>GEOLOGIA</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n"/>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
-      <c r="F7" s="2" t="n"/>
-      <c r="G7" s="2" t="n"/>
-      <c r="H7" s="2" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Geologia</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
+          <t>Estruturas</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Estagiário/Projetista</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>1,44</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>GEOMETRIA</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
-      <c r="F9" s="2" t="n"/>
-      <c r="G9" s="2" t="n"/>
-      <c r="H9" s="2" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Geometria</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>teste9</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>0,38</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>0,76</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>0,38</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>0,38</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>0,38</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>1,50</t>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>1,52</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A5:H5"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -880,7 +1008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,9 +1021,7 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="9" customWidth="1" min="8" max="8"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -926,20 +1052,10 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Mar/24</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Apr/24</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
           <t>H.mês</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Fonte de Dados para o Gráfico</t>
         </is>
@@ -956,14 +1072,12 @@
       <c r="D2" s="2" t="n"/>
       <c r="E2" s="2" t="n"/>
       <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="L2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Mês</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Total Decimal</t>
         </is>
@@ -982,40 +1096,30 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>teste1</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>0,62</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>0,62</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>0,78</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>3,12</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
+          <t>1,25</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Cargo/Subcontrato</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="K3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1027,46 +1131,36 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>testr1</t>
+          <t>teste3</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>0,34</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>0,34</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>0,78</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>0,78</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>3,12</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
+          <t>0,69</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>Jan/24</t>
         </is>
       </c>
-      <c r="M4" t="n">
-        <v>2.68</v>
+      <c r="K4" t="n">
+        <v>1.72</v>
       </c>
     </row>
     <row r="5">
@@ -1080,15 +1174,13 @@
       <c r="D5" s="2" t="n"/>
       <c r="E5" s="2" t="n"/>
       <c r="F5" s="2" t="n"/>
-      <c r="G5" s="2" t="n"/>
-      <c r="H5" s="2" t="n"/>
-      <c r="L5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Feb/24</t>
         </is>
       </c>
-      <c r="M5" t="n">
-        <v>2.68</v>
+      <c r="K5" t="n">
+        <v>1.72</v>
       </c>
     </row>
     <row r="6">
@@ -1099,12 +1191,12 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>teste7</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -1119,154 +1211,46 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>0,38</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>0,38</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>1,50</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Mar/24</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>2.68</v>
+          <t>0,75</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>GEOLOGIA</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n"/>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
-      <c r="F7" s="2" t="n"/>
-      <c r="G7" s="2" t="n"/>
-      <c r="H7" s="2" t="n"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Apr/24</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>2.68</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Geologia</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
+          <t>Estruturas</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Estagiário/Projetista</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>0,36</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>1,44</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>GEOMETRIA</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
-      <c r="F9" s="2" t="n"/>
-      <c r="G9" s="2" t="n"/>
-      <c r="H9" s="2" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Geometria</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>teste9</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>0,38</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>0,38</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>0,38</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>0,38</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>1,50</t>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>0,75</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A5:H5"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -1279,14 +1263,251 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Disciplina</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cargo/Subcontrato</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Funcionário</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Feb/24</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mar/24</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>H.mês</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Fonte de Dados para o Gráfico</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>DRENAGEM</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Mês</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Total Decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Drenagem</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>teste1</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>0,75</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Cargo/Subcontrato</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Drenagem</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>teste3</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>1,56</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>1,56</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>3,12</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Feb/24</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>ESTRUTURAS</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" s="2" t="n"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Mar/24</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Estruturas</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>teste7</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>0,47</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>0,47</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>0,94</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Estruturas</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>teste9</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>0,77</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>